<commit_message>
Started looking at alternate solution
</commit_message>
<xml_diff>
--- a/CH-078 Extract from Text 2.xlsx
+++ b/CH-078 Extract from Text 2.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C847FB6A-D239-41B1-9FEE-6C0985F243E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FFF7C9-A315-4085-A3CD-A18CC88DDEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Alt!$B$7:$B$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$7:$B$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Text</t>
   </si>
@@ -69,6 +93,30 @@
   </si>
   <si>
     <t>The event will take place on 15/06/2024 at 14:20, which is a Saturday. Please RSVP by June 10, 2024. Our office will be closed from July 1st to July 5th, 2024, for the holiday. The deadline for submissions is 2024-08-20 at 12:00. Mark your calendars for September 15, 2024, for the annual conference. The cost is between  2000 to 2020 $. We look forward to seeing you there!</t>
+  </si>
+  <si>
+    <t>The event will take place on 15/06/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> at 14:20, which is a Saturday. Please RSVP by June 10, 2024</t>
+  </si>
+  <si>
+    <t>. Our office will be closed from July 1st to July 5th, 2024</t>
+  </si>
+  <si>
+    <t>, for the holiday. The deadline for submissions is 2024-08-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> at 12:00. Mark your calendars for September 15, 2024</t>
+  </si>
+  <si>
+    <t>, for the annual conference. The cost is between  2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $. We look forward to seeing you there!</t>
   </si>
 </sst>
 </file>
@@ -857,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -1019,4 +1067,262 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342666E0-3245-4ABB-8AC1-D9156918A5A4}">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.69921875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="147.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="str" cm="1">
+        <f t="array" ref="D5:D9">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),
+     _xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
+     _xlfn.TOCOL(
+           _xlfn.IFNA(_xlfn.REGEXREPLACE(_xlpm.y,".*?("&amp;_xlfn.TEXTJOIN("|",,TEXT(_xlfn.SEQUENCE(12)*29,"mmmm"))&amp;")","$1",1),
+           _xlfn.IFS(LEN(--_xlpm.d)&lt;LEN(_xlpm.d),_xlpm.d)),3
+          )
+     )</f>
+        <v>15/06/2024</v>
+      </c>
+      <c r="F5" s="3" t="str" cm="1">
+        <f t="array" ref="F5:F12">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),
+     _xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
+     _xlpm.d
+     )</f>
+        <v>15/06/2024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <v>June 10, 2024</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v>July 1st to July 5th, 2024</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <v>2024-08-20</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <v>2024-08-20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v>September 15, 2024</v>
+      </c>
+      <c r="F9" s="3" t="str">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="F10" s="3" t="str">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="F11" s="3" t="str">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="F12" s="3" t="str">
+        <v>there!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="5" t="str" cm="1">
+        <f t="array" ref="B14:B18">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),_xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
+_xlfn.TOCOL(_xlfn.IFNA(
+           _xlfn.REGEXREPLACE(_xlpm.y,".*?("&amp;_xlfn.TEXTJOIN("|",,TEXT(_xlfn.SEQUENCE(12)*29,"mmmm"))&amp;")","$1",1),
+           _xlfn.IFS(LEN(--_xlpm.d)&lt;LEN(_xlpm.d),_xlpm.d)),3)
+    )</f>
+        <v>15/06/2024</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5" t="str">
+        <v>June 10, 2024</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5" t="str">
+        <v>July 1st to July 5th, 2024</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="5" t="str">
+        <v>2024-08-20</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5" t="str">
+        <v>September 15, 2024</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="2"/>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="2"/>
+      <c r="F20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="2"/>
+      <c r="F21" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started looking at 2nd alternate solution
</commit_message>
<xml_diff>
--- a/CH-078 Extract from Text 2.xlsx
+++ b/CH-078 Extract from Text 2.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FFF7C9-A315-4085-A3CD-A18CC88DDEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE57A62-E396-45CC-AD3B-87247CA82FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Alt!$B$7:$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$B$7:$B$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$7:$B$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>Text</t>
   </si>
@@ -1073,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342666E0-3245-4ABB-8AC1-D9156918A5A4}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1325,4 +1327,283 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F487ED29-806B-47E0-8917-55DB50EE0611}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.69921875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="53.296875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="147.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5" t="str" cm="1">
+        <f t="array" ref="B15:B19">_xlfn.LET(
+_xlpm.d,_xlfn.TEXTSPLIT(B3,,{".",", f"," a","on ","by ","om ","is ","or "}),
+_xlpm.e,_xlfn._xlws.FILTER(_xlpm.d,IFERROR(FIND(2024,_xlpm.d),)),
+_xlfn.SEQUENCE(ROWS(_xlpm.e))&amp;". "&amp;_xlpm.e)</f>
+        <v>1. 15/06/2024</v>
+      </c>
+      <c r="D15" s="3" t="str" cm="1">
+        <f t="array" ref="D15:D36">_xlfn.LET(
+_xlpm.d,_xlfn.TEXTSPLIT(B3,,{".",", f"," a","on ","by ","om ","is ","or "}),
+_xlpm.e,_xlfn._xlws.FILTER(_xlpm.d,IFERROR(FIND(2024,_xlpm.d),)),
+_xlpm.d)</f>
+        <v xml:space="preserve">The event will take place </v>
+      </c>
+      <c r="E15" s="3" t="str" cm="1">
+        <f t="array" ref="E15:E19">_xlfn.LET(
+_xlpm.d,_xlfn.TEXTSPLIT(B3,,{".",", f"," a","on ","by ","om ","is ","or "}),
+_xlpm.e,_xlfn._xlws.FILTER(_xlpm.d,IFERROR(FIND(2024,_xlpm.d),)),
+_xlpm.e)</f>
+        <v>15/06/2024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5" t="str">
+        <v>2. June 10, 2024</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <v>15/06/2024</v>
+      </c>
+      <c r="E16" s="3" t="str">
+        <v>June 10, 2024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="5" t="str">
+        <v>3. July 1st to July 5th, 2024</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <v xml:space="preserve">t 14:20, which </v>
+      </c>
+      <c r="E17" s="3" t="str">
+        <v>July 1st to July 5th, 2024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5" t="str">
+        <v>4. 2024-08-20</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <v>a Saturday</v>
+      </c>
+      <c r="E18" s="3" t="str">
+        <v>2024-08-20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5" t="str">
+        <v>5. September 15, 2024</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <v xml:space="preserve"> Please RSVP </v>
+      </c>
+      <c r="E19" s="3" t="str">
+        <v>September 15, 2024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" s="2"/>
+      <c r="D20" s="3" t="str">
+        <v>June 10, 2024</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" s="2"/>
+      <c r="D21" s="3" t="str">
+        <v xml:space="preserve"> Our office will be closed fr</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" s="2"/>
+      <c r="D22" s="3" t="str">
+        <v>July 1st to July 5th, 2024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" s="2"/>
+      <c r="D23" s="3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" s="2"/>
+      <c r="D24" s="3" t="str">
+        <v>the holiday</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" s="2"/>
+      <c r="D25" s="3" t="str">
+        <v xml:space="preserve"> The deadline f</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="2"/>
+      <c r="D26" s="3" t="str">
+        <v xml:space="preserve">submissions </v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="2"/>
+      <c r="D27" s="3" t="str">
+        <v>2024-08-20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="2"/>
+      <c r="D28" s="3" t="str">
+        <v>t 12:00</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" s="2"/>
+      <c r="D29" s="3" t="str">
+        <v xml:space="preserve"> Mark your calendars f</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" s="2"/>
+      <c r="D30" s="3" t="str">
+        <v>September 15, 2024</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31" s="2"/>
+      <c r="D31" s="3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" s="2"/>
+      <c r="D32" s="3" t="str">
+        <v>the</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D33" s="3" t="str">
+        <v>nnual conference</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" s="4"/>
+      <c r="D34" s="3" t="str">
+        <v xml:space="preserve"> The cost </v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D35" s="3" t="str">
+        <v>between  2000 to 2020 $</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" s="2"/>
+      <c r="D36" s="3" t="str">
+        <v xml:space="preserve"> We look forward to seeing you there!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Breaking down for what I want to do
</commit_message>
<xml_diff>
--- a/CH-078 Extract from Text 2.xlsx
+++ b/CH-078 Extract from Text 2.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE57A62-E396-45CC-AD3B-87247CA82FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542E0382-741D-4629-9CBE-3186B95D0D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt" sheetId="2" r:id="rId2"/>
     <sheet name="Alt2" sheetId="3" r:id="rId3"/>
+    <sheet name="MySingleFunction" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Alt!$B$7:$B$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$B$7:$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MySingleFunction!$B$7:$B$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$7:$B$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,9 +45,10 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -56,16 +59,40 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
   <si>
     <t>Text</t>
   </si>
@@ -119,6 +146,21 @@
   </si>
   <si>
     <t xml:space="preserve"> $. We look forward to seeing you there!</t>
+  </si>
+  <si>
+    <t>15/06/2024</t>
+  </si>
+  <si>
+    <t>June 10, 2024</t>
+  </si>
+  <si>
+    <t>July 1st to July 5th, 2024</t>
+  </si>
+  <si>
+    <t>2024-08-20</t>
+  </si>
+  <si>
+    <t>September 15, 2024</t>
   </si>
 </sst>
 </file>
@@ -660,6 +702,77 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <fb t="e">#N/A</fb>
+    <v>6</v>
+    <v>7</v>
+  </rv>
+  <rv s="1">
+    <v>there!</v>
+    <v>2</v>
+    <v>32</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+  <s t="_error">
+    <k n="argument" t="s"/>
+    <k n="errorType" t="i"/>
+    <k n="iftab" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Wisp">
   <a:themeElements>
@@ -1073,47 +1186,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342666E0-3245-4ABB-8AC1-D9156918A5A4}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="42" style="5" customWidth="1"/>
-    <col min="3" max="3" width="20" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.69921875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="3"/>
+    <col min="2" max="2" width="31.5" style="5" customWidth="1"/>
+    <col min="3" max="4" width="64.8984375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="49" style="3" customWidth="1"/>
+    <col min="6" max="6" width="38.796875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="147.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="147.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="str" cm="1">
-        <f t="array" ref="D5:D9">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),
+      <c r="E5" s="5" t="str" cm="1">
+        <f t="array" ref="E5:E9">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),
      _xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
      _xlfn.TOCOL(
            _xlfn.IFNA(_xlfn.REGEXREPLACE(_xlpm.y,".*?("&amp;_xlfn.TEXTJOIN("|",,TEXT(_xlfn.SEQUENCE(12)*29,"mmmm"))&amp;")","$1",1),
@@ -1122,92 +1236,92 @@
      )</f>
         <v>15/06/2024</v>
       </c>
-      <c r="F5" s="3" t="str" cm="1">
-        <f t="array" ref="F5:F12">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),
+      <c r="G5" s="3" t="str" cm="1">
+        <f t="array" ref="G5:G12">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),
      _xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
      _xlpm.d
      )</f>
         <v>15/06/2024</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="5" t="str">
+      <c r="E6" s="5" t="str">
         <v>June 10, 2024</v>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="G6" s="3" t="str">
         <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="2"/>
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="str">
+      <c r="E7" s="5" t="str">
         <v>July 1st to July 5th, 2024</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="G7" s="3" t="str">
         <v>2024</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="str">
+      <c r="E8" s="5" t="str">
         <v>2024-08-20</v>
       </c>
-      <c r="F8" s="3" t="str">
+      <c r="G8" s="3" t="str">
         <v>2024-08-20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5" t="str">
+      <c r="E9" s="5" t="str">
         <v>September 15, 2024</v>
       </c>
-      <c r="F9" s="3" t="str">
+      <c r="G9" s="3" t="str">
         <v>2024</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="F10" s="3" t="str">
+      <c r="E10" s="6"/>
+      <c r="G10" s="3" t="str">
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="F11" s="3" t="str">
+      <c r="E11" s="6"/>
+      <c r="G11" s="3" t="str">
         <v>2020</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
-      <c r="F12" s="3" t="str">
+      <c r="G12" s="3" t="str">
         <v>there!</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="str" cm="1">
         <f t="array" ref="B14:B18">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),_xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
@@ -1217,95 +1331,212 @@
     )</f>
         <v>15/06/2024</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="C14" s="3" t="str" cm="1">
+        <f t="array" ref="C14:C21">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),_xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
+_xlpm.y
+    )</f>
+        <v>The event will take place on 15/06/2024</v>
+      </c>
+      <c r="D14" s="3" t="str" cm="1">
+        <f t="array" ref="D14:D21">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),_xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
+_xlpm.d
+    )</f>
+        <v>15/06/2024</v>
+      </c>
+      <c r="E14" s="3" t="e" cm="1" vm="1">
+        <f t="array" ref="E14:E21">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),_xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
+_xlpm.z,
+_xlfn.REGEXREPLACE(_xlpm.y,".*?("&amp;_xlfn.TEXTJOIN("|",,TEXT(_xlfn.SEQUENCE(12)*29,"mmmm"))&amp;")","$1",1),_xlpm.z
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="3" t="str" cm="1">
+        <f t="array" ref="F14:F21">_xlfn.LET(_xlpm.y,_xlfn.TEXTSPLIT(_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),,"|"),_xlpm.d,_xlfn.TEXTAFTER(_xlpm.y," ",-1),
+_xlpm.d
+)</f>
+        <v>15/06/2024</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
       <c r="B15" s="5" t="str">
         <v>June 10, 2024</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="C15" s="3" t="str">
+        <v xml:space="preserve"> at 14:20, which is a Saturday. Please RSVP by June 10, 2024</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <v>2024</v>
+      </c>
+      <c r="E15" s="3" t="str">
+        <v>June 10, 2024</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <v>2024</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="str">
         <v>July 1st to July 5th, 2024</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="C16" s="3" t="str">
+        <v>. Our office will be closed from July 1st to July 5th, 2024</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <v>2024</v>
+      </c>
+      <c r="E16" s="3" t="str">
+        <v>July 1st to July 5th, 2024</v>
+      </c>
+      <c r="F16" s="3" t="str">
+        <v>2024</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="str">
         <v>2024-08-20</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="C17" s="3" t="str">
+        <v>, for the holiday. The deadline for submissions is 2024-08-20</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <v>2024-08-20</v>
+      </c>
+      <c r="E17" s="3" t="e" vm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="3" t="str">
+        <v>2024-08-20</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="str">
         <v>September 15, 2024</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="C18" s="3" t="str">
+        <v xml:space="preserve"> at 12:00. Mark your calendars for September 15, 2024</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <v>2024</v>
+      </c>
+      <c r="E18" s="3" t="str">
+        <v>September 15, 2024</v>
+      </c>
+      <c r="F18" s="3" t="str">
+        <v>2024</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
-      <c r="F19" s="3" t="s">
+      <c r="C19" s="3" t="str">
+        <v>, for the annual conference. The cost is between  2000</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <v>2000</v>
+      </c>
+      <c r="E19" s="3" t="e" vm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="F19" s="3" t="str">
+        <v>2000</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
-      <c r="F20" s="3" t="s">
+      <c r="C20" s="3" t="str">
+        <v xml:space="preserve"> to 2020</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <v>2020</v>
+      </c>
+      <c r="E20" s="3" t="e" vm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="F20" s="3" t="str">
+        <v>2020</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="2"/>
-      <c r="F21" s="3" t="s">
+      <c r="C21" s="3" t="str">
+        <v xml:space="preserve"> $. We look forward to seeing you there!</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <v>there!</v>
+      </c>
+      <c r="E21" s="3" t="e" vm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="F21" s="3" t="str">
+        <v>there!</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C25" s="3" t="str" cm="1">
+        <f t="array" ref="C25">".*?("&amp;_xlfn.TEXTJOIN("|",,TEXT(_xlfn.SEQUENCE(12)*29,"mmmm"))&amp;")"</f>
+        <v>.*?(January|February|March|April|May|June|July|August|September|October|November|December)</v>
+      </c>
+      <c r="E25" s="3" t="str" cm="1">
+        <f t="array" ref="E25">_xlfn.TEXTJOIN("|",,TEXT(_xlfn.SEQUENCE(12)*29,"mmmm"))&amp;")"</f>
+        <v>January|February|March|April|May|June|July|August|September|October|November|December)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="2"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.4">
@@ -1333,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F487ED29-806B-47E0-8917-55DB50EE0611}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="C33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -1606,4 +1837,301 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A49B2E-9711-4C28-B7B5-181A86EC51D8}">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="57.8984375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.69921875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="147.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="5" t="str">
+        <f>_xlfn.LET(_xlpm.y,_xlfn.REGEXREPLACE(B3,"[\d/-]{4,}","$0|"),
+     _xlpm.y)</f>
+        <v>The event will take place on 15/06/2024| at 14:20, which is a Saturday. Please RSVP by June 10, 2024|. Our office will be closed from July 1st to July 5th, 2024|, for the holiday. The deadline for submissions is 2024-08-20| at 12:00. Mark your calendars for September 15, 2024|, for the annual conference. The cost is between  2000| to 2020| $. We look forward to seeing you there!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5" t="str" cm="1">
+        <f t="array" ref="B15:B22">_xlfn.TEXTSPLIT(B14,,"|")</f>
+        <v>The event will take place on 15/06/2024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5" t="str">
+        <v xml:space="preserve"> at 14:20, which is a Saturday. Please RSVP by June 10, 2024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="5" t="str">
+        <v>. Our office will be closed from July 1st to July 5th, 2024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5" t="str">
+        <v>, for the holiday. The deadline for submissions is 2024-08-20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5" t="str">
+        <v xml:space="preserve"> at 12:00. Mark your calendars for September 15, 2024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5" t="str">
+        <v>, for the annual conference. The cost is between  2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="2"/>
+      <c r="B21" s="5" t="str">
+        <v xml:space="preserve"> to 2020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="2"/>
+      <c r="B22" s="5" t="str">
+        <v xml:space="preserve"> $. We look forward to seeing you there!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="2"/>
+      <c r="B24" s="5" t="str" cm="1">
+        <f t="array" ref="B24:B31">_xlfn.TEXTAFTER(_xlfn.ANCHORARRAY(B15)," ",-1)</f>
+        <v>15/06/2024</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="5" t="str">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="2"/>
+      <c r="B26" s="5" t="str">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="2"/>
+      <c r="B27" s="5" t="str">
+        <v>2024-08-20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="2"/>
+      <c r="B28" s="5" t="str">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="2"/>
+      <c r="B29" s="5" t="str">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="5" t="str">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="2"/>
+      <c r="B31" s="5" t="str">
+        <v>there!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B33" s="5" t="str" cm="1">
+        <f t="array" ref="B33:B40">_xlfn.LET(_xlpm.d,_xlfn.TEXTAFTER(_xlfn.ANCHORARRAY(B15)," ",-1),
+_xlfn.IFNA(
+           _xlfn.REGEXREPLACE(_xlfn.ANCHORARRAY(B15),".*?("&amp;_xlfn.TEXTJOIN("|",,TEXT(_xlfn.SEQUENCE(12)*29,"mmmm"))&amp;")","$1",1),
+           _xlfn.IFS(LEN(--_xlpm.d)&lt;LEN(_xlpm.d),_xlpm.d))
+)</f>
+        <v>15/06/2024</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5" t="str">
+        <v>June 10, 2024</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B35" s="5" t="str">
+        <v>July 1st to July 5th, 2024</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" s="2"/>
+      <c r="B36" s="5" t="str">
+        <v>2024-08-20</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" s="2"/>
+      <c r="B37" s="5" t="str">
+        <v>September 15, 2024</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="2"/>
+      <c r="B38" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" s="2"/>
+      <c r="B39" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B40" s="5" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B42" s="5" t="str" cm="1">
+        <f t="array" ref="B42:B46">_xlfn.TOCOL(_xlfn.ANCHORARRAY(B33),3)</f>
+        <v>15/06/2024</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B43" s="5" t="str">
+        <v>June 10, 2024</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B44" s="5" t="str">
+        <v>July 1st to July 5th, 2024</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B45" s="5" t="str">
+        <v>2024-08-20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B46" s="5" t="str">
+        <v>September 15, 2024</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>